<commit_message>
added all data into pythoncsv file
</commit_message>
<xml_diff>
--- a/excel_csv/final_data.xlsx
+++ b/excel_csv/final_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lawrencetang/Desktop/Internships:Research/UROP/oilresearch/excel_csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7754D4-A5A8-EA45-89FE-1DF62A7EBF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1095960A-496F-034F-99E8-4557CC75C3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68640" yWindow="500" windowWidth="38400" windowHeight="23500" activeTab="2" xr2:uid="{0CDE113E-35AD-2643-904C-47F0C01455AB}"/>
+    <workbookView xWindow="68640" yWindow="500" windowWidth="38400" windowHeight="23500" activeTab="4" xr2:uid="{0CDE113E-35AD-2643-904C-47F0C01455AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
   <si>
     <t>Bloomberg</t>
   </si>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>python imports last 5 day rolling average</t>
+  </si>
+  <si>
+    <t>Python imports the data from the tabs Bloomberg, Statista, Treasury, Investing.com and spits out the following data and chart</t>
+  </si>
+  <si>
+    <t>THIS IS IMPORTED INTO PYTHON (imported via API, data just shown here for visibility)</t>
   </si>
 </sst>
 </file>
@@ -748,10 +754,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9FE935F-3708-A547-8EC8-4BACEA2299B7}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -759,6 +765,11 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -770,7 +781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C491D87-F346-CA48-BF83-3B74F4392A2D}">
   <dimension ref="A1:F533"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
@@ -15482,7 +15493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FA34E8-AF23-5B46-BA07-871AB5EF464C}">
   <dimension ref="A1:H513"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -26711,7 +26722,7 @@
   <dimension ref="A1:E532"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26768,7 +26779,7 @@
         <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
changed plot axis names
</commit_message>
<xml_diff>
--- a/excel_csv/final_data.xlsx
+++ b/excel_csv/final_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lawrencetang/Desktop/Internships:Research/UROP/oilresearch/excel_csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1470AC-5FA7-124F-9B96-A1E9CD0BEF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC05E574-022D-2646-83BE-AC6C4AF873C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{0CDE113E-35AD-2643-904C-47F0C01455AB}"/>
+    <workbookView xWindow="30220" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{0CDE113E-35AD-2643-904C-47F0C01455AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="5" r:id="rId1"/>
@@ -21,11 +21,6 @@
     <sheet name="Treasury" sheetId="3" r:id="rId6"/>
     <sheet name="Datastream" sheetId="8" r:id="rId7"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Datastream!$A$8:$A$539</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Datastream!$I$7</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Datastream!$I$8:$I$539</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="72">
   <si>
     <t>Bloomberg</t>
   </si>
@@ -271,6 +266,21 @@
   </si>
   <si>
     <t>3. plot the data (in series.py and average.py), did not do matching, instead just went as far as data could, interpolated data linearly in between if missing a date</t>
+  </si>
+  <si>
+    <t>Note: Last 5 day rolling average</t>
+  </si>
+  <si>
+    <t>Sources:</t>
+  </si>
+  <si>
+    <t>Bloomberg (subscription required)</t>
+  </si>
+  <si>
+    <t>Datastream (subscription required)</t>
+  </si>
+  <si>
+    <t>Neste</t>
   </si>
 </sst>
 </file>
@@ -16166,23 +16176,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>162560</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>81280</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>246418</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>75821</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>182880</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>217909</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>379</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="12" name="Picture 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2D0D0D3-B539-7DF4-DAD8-FD246DD71A41}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB80F152-3EEC-384A-C94E-6785A966420B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16198,8 +16208,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16022320" y="14102080"/>
-          <a:ext cx="9144000" cy="4572000"/>
+          <a:off x="7127164" y="4037463"/>
+          <a:ext cx="7772400" cy="3886200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16210,23 +16220,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>680720</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>71120</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>360149</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>208507</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>751840</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>162560</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>626281</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>133065</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{126F5D0B-0E1E-8FCD-40B2-67E36DFA4195}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D6BE0C2-6EEF-FD6D-8627-DA082920EB25}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16242,8 +16252,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6664960" y="14091920"/>
-          <a:ext cx="9123680" cy="4561840"/>
+          <a:off x="16415224" y="9382835"/>
+          <a:ext cx="7772400" cy="3886200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16255,22 +16265,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>142240</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>162560</xdr:rowOff>
+      <xdr:colOff>284328</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>113731</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>314960</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>550460</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>38289</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="14" name="Picture 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBC32D9D-242B-0916-B60C-0D93FEF2A753}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02BA135F-AA37-415C-6E05-BE72FAEDCFBB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16286,8 +16296,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16002000" y="8900160"/>
-          <a:ext cx="9225280" cy="4612640"/>
+          <a:off x="16339403" y="4075373"/>
+          <a:ext cx="7772400" cy="3886200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16298,23 +16308,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>40640</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>758209</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>325120</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>10160</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>718630</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>133065</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
+        <xdr:cNvPr id="15" name="Picture 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82A45714-2229-AA34-AFB3-FE70A9DA22B2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEAB2958-C30E-031A-4866-94080F6E1A94}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16330,8 +16340,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15951200" y="3698240"/>
-          <a:ext cx="9286240" cy="4643120"/>
+          <a:off x="7638955" y="14595522"/>
+          <a:ext cx="7772400" cy="3886200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16342,23 +16352,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>782320</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>358179</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>7431</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>162560</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>624310</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>140496</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
+        <xdr:cNvPr id="16" name="Picture 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40B32A21-30AB-719F-B70A-962E3FD8F45A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8904ADBE-79AD-C365-F1B0-759224B71A37}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16374,8 +16384,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6766560" y="3749040"/>
-          <a:ext cx="9083040" cy="4541520"/>
+          <a:off x="16217939" y="14231431"/>
+          <a:ext cx="7672771" cy="3790665"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16883,14 +16893,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9FE935F-3708-A547-8EC8-4BACEA2299B7}">
   <dimension ref="A1:V496"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="125" zoomScaleNormal="108" workbookViewId="0">
-      <pane ySplit="12" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T8" sqref="T8"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="125" workbookViewId="0">
+      <pane ySplit="12" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L97" sqref="L97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="11" max="11" width="5.83203125" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" customWidth="1"/>
+    <col min="13" max="13" width="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
@@ -18355,7 +18368,7 @@
         <v>-33.445999999999998</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>44659</v>
       </c>
@@ -18375,7 +18388,7 @@
         <v>-35.235999999999997</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>44662</v>
       </c>
@@ -18395,7 +18408,7 @@
         <v>-35.643999999999998</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>44663</v>
       </c>
@@ -18415,7 +18428,7 @@
         <v>-35.79</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>44664</v>
       </c>
@@ -18435,7 +18448,7 @@
         <v>-36.567999999999998</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>44665</v>
       </c>
@@ -18455,7 +18468,7 @@
         <v>-37.058999999999997</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>44670</v>
       </c>
@@ -18475,7 +18488,7 @@
         <v>-38.301000000000002</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>44671</v>
       </c>
@@ -18495,7 +18508,7 @@
         <v>-38.314999999999998</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>44672</v>
       </c>
@@ -18515,7 +18528,7 @@
         <v>-37.914999999999999</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>44673</v>
       </c>
@@ -18535,7 +18548,7 @@
         <v>-37.396999999999998</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>44676</v>
       </c>
@@ -18555,7 +18568,7 @@
         <v>-37.485999999999997</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>44677</v>
       </c>
@@ -18575,7 +18588,7 @@
         <v>-37.51</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>44678</v>
       </c>
@@ -18595,7 +18608,7 @@
         <v>-37.405999999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>44679</v>
       </c>
@@ -18615,7 +18628,7 @@
         <v>-37.380000000000003</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>44680</v>
       </c>
@@ -18634,8 +18647,11 @@
       <c r="F94">
         <v>-36.774000000000001</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J94" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>44684</v>
       </c>
@@ -18654,8 +18670,23 @@
       <c r="F95">
         <v>-34.713999999999999</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J95" t="s">
+        <v>68</v>
+      </c>
+      <c r="K95" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="L95" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="M95" t="s">
+        <v>69</v>
+      </c>
+      <c r="N95" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>44685</v>
       </c>
@@ -26676,8 +26707,12 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K95" r:id="rId1" xr:uid="{4B1FF654-60A0-A34D-B88B-23FD282DA53A}"/>
+    <hyperlink ref="L95" r:id="rId2" xr:uid="{B0A9BD93-DC67-954E-94F1-DCD51205FF8C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -26686,8 +26721,8 @@
   <dimension ref="A1:I534"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q16" sqref="Q16"/>
+      <pane ySplit="7" topLeftCell="A497" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -37311,7 +37346,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -45300,8 +45335,8 @@
   <dimension ref="A1:G510"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
+      <pane ySplit="8" topLeftCell="A407" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -60618,8 +60653,8 @@
   <dimension ref="A1:K539"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O33" sqref="O33"/>
+      <pane ySplit="7" topLeftCell="A472" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>